<commit_message>
upgrading to the latest SHAFT_Engine version
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/Google/SimpleSearch.xlsx
+++ b/src/test/resources/TestDataFiles/Google/SimpleSearch.xlsx
@@ -47,7 +47,7 @@
     <t xml:space="preserve">Expected First Search Result Link</t>
   </si>
   <si>
-    <t xml:space="preserve">https://github.com/MohabMohie/SHAFT_ENGINE</t>
+    <t xml:space="preserve">SHAFT_ENGINE</t>
   </si>
   <si>
     <t xml:space="preserve">Supported Browser Types</t>
@@ -72,7 +72,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -112,13 +112,6 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -178,7 +171,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -193,10 +186,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -292,7 +281,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -333,7 +322,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -345,9 +334,6 @@
   <mergeCells count="1">
     <mergeCell ref="A2:C2"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="https://github.com/MohabMohie/SHAFT_ENGINE"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -376,7 +362,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>